<commit_message>
Avance final del día
Ultimo avance del día con algunos graficos terminados
</commit_message>
<xml_diff>
--- a/datasets/junior.xlsx
+++ b/datasets/junior.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\analisis_liga_aguila\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8B8088-1048-4A44-87C0-64CD7785C326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C111009-58DA-4873-BFAB-8F0FAE71A04D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21CA4667-EA8C-4557-A323-B5300215427C}"/>
   </bookViews>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC54474-AE53-4F1E-9BC7-10E326CB4E52}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,9 @@
     <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1603,10 +1605,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1916,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>3</v>

</xml_diff>